<commit_message>
Refactoring water-types to function, added test, usage example comments and descriptions
</commit_message>
<xml_diff>
--- a/water_facies.xlsx
+++ b/water_facies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,42 +434,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sample</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>pH</t>
+          <t>MCation</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>MCation</t>
+          <t>MAnion</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>MAnion</t>
+          <t>Salinity</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Salinity</t>
+          <t>Alkalinity</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Alkalinity</t>
+          <t>BEX</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>BEX</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Code</t>
         </is>
@@ -477,361 +467,331 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>5.52</v>
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Mg</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mg</t>
+          <t>SO4</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SO4</t>
+          <t>g</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
           <t>*</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>g*MgSO4</t>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>g*-MgSO4</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>6.03</v>
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Cl</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Cl</t>
+          <t>g</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
           <t>*</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>g*NaCl</t>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>g*-NaCl</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>6.58</v>
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Ca</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ca</t>
+          <t>MIX</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>MIX</t>
+          <t>g</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
           <t>*</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>g*CaMIX</t>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>g*-CaMIX</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>6.38</v>
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ca</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ca</t>
+          <t>HCO3</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>HCO3</t>
+          <t>g</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
           <t>*</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>g*CaHCO3</t>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>g*-CaHCO3</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>7.13</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Ca</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ca</t>
+          <t>HCO3</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>HCO3</t>
+          <t>g</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>+</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>g3CaHCO3+</t>
+          <t>g3-CaHCO3+</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>7.53</v>
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ca</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ca</t>
+          <t>MIX</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>MIX</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>+</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>F2CaMIX+</t>
+          <t>F2-CaMIX+</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7.74</v>
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Ca</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ca</t>
+          <t>NO3</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>NO3</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>+</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>F2CaNO3+</t>
+          <t>F2-CaNO3+</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>7.68</v>
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ca</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ca</t>
+          <t>HCO3</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>HCO3</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>F2CaHCO3</t>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>F2-CaHCO3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>7.48</v>
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Ca</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ca</t>
+          <t>MIX</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>MIX</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>+</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>F3CaMIX+</t>
+          <t>F3-CaMIX+</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>8.16</v>
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Ca</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ca</t>
+          <t>NO3</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>NO3</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>+</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>F1CaNO3+</t>
+          <t>F1-CaNO3+</t>
         </is>
       </c>
     </row>

</xml_diff>